<commit_message>
Project code + scripts (data excluded)
</commit_message>
<xml_diff>
--- a/Machine_Learning_Project_Checklist.xlsx
+++ b/Machine_Learning_Project_Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abiga\source\repos\MachineLearning\MachineLearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA88013-E746-4D7A-BBF0-B310569DD21A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7810341-FCC1-4420-98AA-D7CC199550D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12390" yWindow="-14550" windowWidth="21600" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ML Project Checklist" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="52">
   <si>
     <t>Phase</t>
   </si>
@@ -533,7 +533,7 @@
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -605,6 +605,9 @@
       <c r="B6" t="s">
         <v>9</v>
       </c>
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -613,6 +616,9 @@
       <c r="B7" t="s">
         <v>10</v>
       </c>
+      <c r="C7" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -621,6 +627,9 @@
       <c r="B8" t="s">
         <v>12</v>
       </c>
+      <c r="C8" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -629,6 +638,9 @@
       <c r="B9" t="s">
         <v>13</v>
       </c>
+      <c r="C9" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -636,6 +648,9 @@
       </c>
       <c r="B10" t="s">
         <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Update presentation and project checklist
</commit_message>
<xml_diff>
--- a/Machine_Learning_Project_Checklist.xlsx
+++ b/Machine_Learning_Project_Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abiga\source\repos\MachineLearning\MachineLearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7810341-FCC1-4420-98AA-D7CC199550D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0618CF-1D6A-4EC3-8352-E49E9AE3E9C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
   <si>
     <t>Phase</t>
   </si>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -532,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -660,6 +663,9 @@
       <c r="B11" t="s">
         <v>16</v>
       </c>
+      <c r="C11" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -668,6 +674,9 @@
       <c r="B12" t="s">
         <v>17</v>
       </c>
+      <c r="C12" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -676,6 +685,9 @@
       <c r="B13" t="s">
         <v>19</v>
       </c>
+      <c r="C13" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -684,6 +696,9 @@
       <c r="B14" t="s">
         <v>20</v>
       </c>
+      <c r="C14" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -692,6 +707,9 @@
       <c r="B15" t="s">
         <v>21</v>
       </c>
+      <c r="C15" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -700,40 +718,55 @@
       <c r="B16" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>18</v>
       </c>
       <c r="B17" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>24</v>
       </c>
       <c r="B18" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>24</v>
       </c>
       <c r="B19" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>24</v>
       </c>
       <c r="B20" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -741,7 +774,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -749,7 +782,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -757,7 +790,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -765,7 +798,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -773,7 +806,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -781,7 +814,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -789,7 +822,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -797,7 +830,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -805,7 +838,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -813,7 +846,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -821,7 +854,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
Add project presentation and checklist documents
</commit_message>
<xml_diff>
--- a/Machine_Learning_Project_Checklist.xlsx
+++ b/Machine_Learning_Project_Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abiga\source\repos\MachineLearning\MachineLearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0618CF-1D6A-4EC3-8352-E49E9AE3E9C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE377FDA-59AC-4123-9AF4-6E531FA10978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="53">
   <si>
     <t>Phase</t>
   </si>
@@ -535,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -773,6 +773,9 @@
       <c r="B21" t="s">
         <v>29</v>
       </c>
+      <c r="C21" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
@@ -781,6 +784,9 @@
       <c r="B22" t="s">
         <v>30</v>
       </c>
+      <c r="C22" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
@@ -821,6 +827,9 @@
       <c r="B27" t="s">
         <v>37</v>
       </c>
+      <c r="C27" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
@@ -829,6 +838,9 @@
       <c r="B28" t="s">
         <v>38</v>
       </c>
+      <c r="C28" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
@@ -862,23 +874,29 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>45</v>
       </c>
       <c r="B33" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C33" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>45</v>
       </c>
       <c r="B34" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C34" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>48</v>
       </c>
@@ -886,7 +904,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
Add training pipeline, Flask prediction service, and UI
</commit_message>
<xml_diff>
--- a/Machine_Learning_Project_Checklist.xlsx
+++ b/Machine_Learning_Project_Checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abiga\source\repos\MachineLearning\MachineLearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE377FDA-59AC-4123-9AF4-6E531FA10978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BBD6230-2AEF-4527-AB13-1C85DCEC170B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="53">
   <si>
     <t>Phase</t>
   </si>
@@ -535,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -795,6 +795,9 @@
       <c r="B23" t="s">
         <v>32</v>
       </c>
+      <c r="C23" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
@@ -803,6 +806,9 @@
       <c r="B24" t="s">
         <v>33</v>
       </c>
+      <c r="C24" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
@@ -811,6 +817,9 @@
       <c r="B25" t="s">
         <v>34</v>
       </c>
+      <c r="C25" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
@@ -819,6 +828,9 @@
       <c r="B26" t="s">
         <v>35</v>
       </c>
+      <c r="C26" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
@@ -849,6 +861,9 @@
       <c r="B29" t="s">
         <v>40</v>
       </c>
+      <c r="C29" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
@@ -857,6 +872,9 @@
       <c r="B30" t="s">
         <v>41</v>
       </c>
+      <c r="C30" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
@@ -865,6 +883,9 @@
       <c r="B31" t="s">
         <v>43</v>
       </c>
+      <c r="C31" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
@@ -873,6 +894,9 @@
       <c r="B32" t="s">
         <v>44</v>
       </c>
+      <c r="C32" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
@@ -903,6 +927,9 @@
       <c r="B35" t="s">
         <v>49</v>
       </c>
+      <c r="C35" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
@@ -910,6 +937,9 @@
       </c>
       <c r="B36" t="s">
         <v>50</v>
+      </c>
+      <c r="C36" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>